<commit_message>
Plots Routes so far
</commit_message>
<xml_diff>
--- a/src/path_planning/test_scripts/Testing.xlsx
+++ b/src/path_planning/test_scripts/Testing.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C79"/>
+  <dimension ref="A1:C82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1290,6 +1290,39 @@
         <v>0.1180344612612334</v>
       </c>
     </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>0.009621207843739724</v>
+      </c>
+      <c r="B80" t="n">
+        <v>0.2335480718435533</v>
+      </c>
+      <c r="C80" t="n">
+        <v>0.1699024050833353</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>0.01924044167894088</v>
+      </c>
+      <c r="B81" t="n">
+        <v>0.2316540184638475</v>
+      </c>
+      <c r="C81" t="n">
+        <v>0.1679318969715666</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>0.01924044167894088</v>
+      </c>
+      <c r="B82" t="n">
+        <v>0.2316540184638475</v>
+      </c>
+      <c r="C82" t="n">
+        <v>0.1679318969715666</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
literally hacking the matrix
</commit_message>
<xml_diff>
--- a/src/path_planning/test_scripts/Testing.xlsx
+++ b/src/path_planning/test_scripts/Testing.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2164"/>
+  <dimension ref="A1:C2338"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -24224,6 +24224,1920 @@
         <v>13.50936816150611</v>
       </c>
     </row>
+    <row r="2165">
+      <c r="A2165" t="n">
+        <v>9.747220500373512</v>
+      </c>
+      <c r="B2165" t="n">
+        <v>9.748954268583869</v>
+      </c>
+      <c r="C2165" t="n">
+        <v>16.04746703319188</v>
+      </c>
+    </row>
+    <row r="2166">
+      <c r="A2166" t="n">
+        <v>9.041427085808614</v>
+      </c>
+      <c r="B2166" t="n">
+        <v>9.043119691663314</v>
+      </c>
+      <c r="C2166" t="n">
+        <v>15.98702527626669</v>
+      </c>
+    </row>
+    <row r="2167">
+      <c r="A2167" t="n">
+        <v>8.335633671243716</v>
+      </c>
+      <c r="B2167" t="n">
+        <v>8.337285114742759</v>
+      </c>
+      <c r="C2167" t="n">
+        <v>15.9265835193415</v>
+      </c>
+    </row>
+    <row r="2168">
+      <c r="A2168" t="n">
+        <v>7.629840256678818</v>
+      </c>
+      <c r="B2168" t="n">
+        <v>7.631450537822205</v>
+      </c>
+      <c r="C2168" t="n">
+        <v>15.8661417624163</v>
+      </c>
+    </row>
+    <row r="2169">
+      <c r="A2169" t="n">
+        <v>6.924046842113921</v>
+      </c>
+      <c r="B2169" t="n">
+        <v>6.92561596090165</v>
+      </c>
+      <c r="C2169" t="n">
+        <v>15.80570000549111</v>
+      </c>
+    </row>
+    <row r="2170">
+      <c r="A2170" t="n">
+        <v>6.218253427549023</v>
+      </c>
+      <c r="B2170" t="n">
+        <v>6.219781383981096</v>
+      </c>
+      <c r="C2170" t="n">
+        <v>15.74525824856592</v>
+      </c>
+    </row>
+    <row r="2171">
+      <c r="A2171" t="n">
+        <v>5.512460012984125</v>
+      </c>
+      <c r="B2171" t="n">
+        <v>5.513946807060542</v>
+      </c>
+      <c r="C2171" t="n">
+        <v>15.68481649164073</v>
+      </c>
+    </row>
+    <row r="2172">
+      <c r="A2172" t="n">
+        <v>4.806666598419227</v>
+      </c>
+      <c r="B2172" t="n">
+        <v>4.808112230139987</v>
+      </c>
+      <c r="C2172" t="n">
+        <v>15.62437473471554</v>
+      </c>
+    </row>
+    <row r="2173">
+      <c r="A2173" t="n">
+        <v>4.100873183854329</v>
+      </c>
+      <c r="B2173" t="n">
+        <v>4.102277653219433</v>
+      </c>
+      <c r="C2173" t="n">
+        <v>15.56393297779034</v>
+      </c>
+    </row>
+    <row r="2174">
+      <c r="A2174" t="n">
+        <v>3.395079769289431</v>
+      </c>
+      <c r="B2174" t="n">
+        <v>3.396443076298878</v>
+      </c>
+      <c r="C2174" t="n">
+        <v>15.50349122086515</v>
+      </c>
+    </row>
+    <row r="2175">
+      <c r="A2175" t="n">
+        <v>2.689286354724533</v>
+      </c>
+      <c r="B2175" t="n">
+        <v>2.690608499378324</v>
+      </c>
+      <c r="C2175" t="n">
+        <v>15.44304946393996</v>
+      </c>
+    </row>
+    <row r="2176">
+      <c r="A2176" t="n">
+        <v>1.983492940159636</v>
+      </c>
+      <c r="B2176" t="n">
+        <v>1.984773922457769</v>
+      </c>
+      <c r="C2176" t="n">
+        <v>15.38260770701477</v>
+      </c>
+    </row>
+    <row r="2177">
+      <c r="A2177" t="n">
+        <v>1.277699525594738</v>
+      </c>
+      <c r="B2177" t="n">
+        <v>1.278939345537215</v>
+      </c>
+      <c r="C2177" t="n">
+        <v>15.32216595008958</v>
+      </c>
+    </row>
+    <row r="2178">
+      <c r="A2178" t="n">
+        <v>0.5719061110298396</v>
+      </c>
+      <c r="B2178" t="n">
+        <v>0.5731047686166604</v>
+      </c>
+      <c r="C2178" t="n">
+        <v>15.26172419316438</v>
+      </c>
+    </row>
+    <row r="2179">
+      <c r="A2179" t="n">
+        <v>-0.1338873035350584</v>
+      </c>
+      <c r="B2179" t="n">
+        <v>-0.132729808303894</v>
+      </c>
+      <c r="C2179" t="n">
+        <v>15.20128243623919</v>
+      </c>
+    </row>
+    <row r="2180">
+      <c r="A2180" t="n">
+        <v>-0.8396807180999564</v>
+      </c>
+      <c r="B2180" t="n">
+        <v>-0.8385643852244485</v>
+      </c>
+      <c r="C2180" t="n">
+        <v>15.140840679314</v>
+      </c>
+    </row>
+    <row r="2181">
+      <c r="A2181" t="n">
+        <v>-1.545474132664854</v>
+      </c>
+      <c r="B2181" t="n">
+        <v>-1.544398962145003</v>
+      </c>
+      <c r="C2181" t="n">
+        <v>15.08039892238881</v>
+      </c>
+    </row>
+    <row r="2182">
+      <c r="A2182" t="n">
+        <v>-2.251267547229752</v>
+      </c>
+      <c r="B2182" t="n">
+        <v>-2.250233539065557</v>
+      </c>
+      <c r="C2182" t="n">
+        <v>15.01995716546362</v>
+      </c>
+    </row>
+    <row r="2183">
+      <c r="A2183" t="n">
+        <v>-2.95706096179465</v>
+      </c>
+      <c r="B2183" t="n">
+        <v>-2.956068115986112</v>
+      </c>
+      <c r="C2183" t="n">
+        <v>14.95951540853843</v>
+      </c>
+    </row>
+    <row r="2184">
+      <c r="A2184" t="n">
+        <v>-3.662854376359548</v>
+      </c>
+      <c r="B2184" t="n">
+        <v>-3.661902692906666</v>
+      </c>
+      <c r="C2184" t="n">
+        <v>14.89907365161323</v>
+      </c>
+    </row>
+    <row r="2185">
+      <c r="A2185" t="n">
+        <v>-4.368647790924446</v>
+      </c>
+      <c r="B2185" t="n">
+        <v>-4.36773726982722</v>
+      </c>
+      <c r="C2185" t="n">
+        <v>14.83863189468804</v>
+      </c>
+    </row>
+    <row r="2186">
+      <c r="A2186" t="n">
+        <v>-5.074441205489344</v>
+      </c>
+      <c r="B2186" t="n">
+        <v>-5.073571846747774</v>
+      </c>
+      <c r="C2186" t="n">
+        <v>14.77819013776285</v>
+      </c>
+    </row>
+    <row r="2187">
+      <c r="A2187" t="n">
+        <v>-5.780234620054242</v>
+      </c>
+      <c r="B2187" t="n">
+        <v>-5.779406423668329</v>
+      </c>
+      <c r="C2187" t="n">
+        <v>14.71774838083766</v>
+      </c>
+    </row>
+    <row r="2188">
+      <c r="A2188" t="n">
+        <v>-6.48602803461914</v>
+      </c>
+      <c r="B2188" t="n">
+        <v>-6.485241000588883</v>
+      </c>
+      <c r="C2188" t="n">
+        <v>14.65730662391247</v>
+      </c>
+    </row>
+    <row r="2189">
+      <c r="A2189" t="n">
+        <v>-7.191821449184038</v>
+      </c>
+      <c r="B2189" t="n">
+        <v>-7.191075577509437</v>
+      </c>
+      <c r="C2189" t="n">
+        <v>14.59686486698728</v>
+      </c>
+    </row>
+    <row r="2190">
+      <c r="A2190" t="n">
+        <v>-7.897614863748935</v>
+      </c>
+      <c r="B2190" t="n">
+        <v>-7.896910154429992</v>
+      </c>
+      <c r="C2190" t="n">
+        <v>14.53642311006208</v>
+      </c>
+    </row>
+    <row r="2191">
+      <c r="A2191" t="n">
+        <v>-8.603408278313834</v>
+      </c>
+      <c r="B2191" t="n">
+        <v>-8.602744731350546</v>
+      </c>
+      <c r="C2191" t="n">
+        <v>14.47598135313689</v>
+      </c>
+    </row>
+    <row r="2192">
+      <c r="A2192" t="n">
+        <v>-9.309201692878732</v>
+      </c>
+      <c r="B2192" t="n">
+        <v>-9.308579308271101</v>
+      </c>
+      <c r="C2192" t="n">
+        <v>14.4155395962117</v>
+      </c>
+    </row>
+    <row r="2193">
+      <c r="A2193" t="n">
+        <v>-10.01499510744363</v>
+      </c>
+      <c r="B2193" t="n">
+        <v>-10.01441388519166</v>
+      </c>
+      <c r="C2193" t="n">
+        <v>14.35509783928651</v>
+      </c>
+    </row>
+    <row r="2194">
+      <c r="A2194" t="n">
+        <v>-10.72078852200853</v>
+      </c>
+      <c r="B2194" t="n">
+        <v>-10.72024846211221</v>
+      </c>
+      <c r="C2194" t="n">
+        <v>14.29465608236132</v>
+      </c>
+    </row>
+    <row r="2195">
+      <c r="A2195" t="n">
+        <v>-11.42658193657343</v>
+      </c>
+      <c r="B2195" t="n">
+        <v>-11.42608303903277</v>
+      </c>
+      <c r="C2195" t="n">
+        <v>14.23421432543613</v>
+      </c>
+    </row>
+    <row r="2196">
+      <c r="A2196" t="n">
+        <v>-12.13237535113832</v>
+      </c>
+      <c r="B2196" t="n">
+        <v>-12.13191761595332</v>
+      </c>
+      <c r="C2196" t="n">
+        <v>14.17377256851094</v>
+      </c>
+    </row>
+    <row r="2197">
+      <c r="A2197" t="n">
+        <v>-12.83816876570322</v>
+      </c>
+      <c r="B2197" t="n">
+        <v>-12.83775219287388</v>
+      </c>
+      <c r="C2197" t="n">
+        <v>14.11333081158575</v>
+      </c>
+    </row>
+    <row r="2198">
+      <c r="A2198" t="n">
+        <v>-13.54396218026812</v>
+      </c>
+      <c r="B2198" t="n">
+        <v>-13.54358676979443</v>
+      </c>
+      <c r="C2198" t="n">
+        <v>14.05288905466056</v>
+      </c>
+    </row>
+    <row r="2199">
+      <c r="A2199" t="n">
+        <v>-14.24975559483302</v>
+      </c>
+      <c r="B2199" t="n">
+        <v>-14.24942134671499</v>
+      </c>
+      <c r="C2199" t="n">
+        <v>13.99244729773537</v>
+      </c>
+    </row>
+    <row r="2200">
+      <c r="A2200" t="n">
+        <v>-14.95554900939791</v>
+      </c>
+      <c r="B2200" t="n">
+        <v>-14.95525592363554</v>
+      </c>
+      <c r="C2200" t="n">
+        <v>13.93200554081018</v>
+      </c>
+    </row>
+    <row r="2201">
+      <c r="A2201" t="n">
+        <v>-15.66134242396281</v>
+      </c>
+      <c r="B2201" t="n">
+        <v>-15.6610905005561</v>
+      </c>
+      <c r="C2201" t="n">
+        <v>13.87156378388499</v>
+      </c>
+    </row>
+    <row r="2202">
+      <c r="A2202" t="n">
+        <v>-16.36713583852771</v>
+      </c>
+      <c r="B2202" t="n">
+        <v>-16.36692507747665</v>
+      </c>
+      <c r="C2202" t="n">
+        <v>13.81112202695979</v>
+      </c>
+    </row>
+    <row r="2203">
+      <c r="A2203" t="n">
+        <v>-17.07292925309261</v>
+      </c>
+      <c r="B2203" t="n">
+        <v>-17.07275965439721</v>
+      </c>
+      <c r="C2203" t="n">
+        <v>13.7506802700346</v>
+      </c>
+    </row>
+    <row r="2204">
+      <c r="A2204" t="n">
+        <v>-17.77872266765751</v>
+      </c>
+      <c r="B2204" t="n">
+        <v>-17.77859423131776</v>
+      </c>
+      <c r="C2204" t="n">
+        <v>13.69023851310941</v>
+      </c>
+    </row>
+    <row r="2205">
+      <c r="A2205" t="n">
+        <v>-18.48451608222241</v>
+      </c>
+      <c r="B2205" t="n">
+        <v>-18.48442880823832</v>
+      </c>
+      <c r="C2205" t="n">
+        <v>13.62979675618422</v>
+      </c>
+    </row>
+    <row r="2206">
+      <c r="A2206" t="n">
+        <v>-19.1903094967873</v>
+      </c>
+      <c r="B2206" t="n">
+        <v>-19.19026338515887</v>
+      </c>
+      <c r="C2206" t="n">
+        <v>13.56935499925903</v>
+      </c>
+    </row>
+    <row r="2207">
+      <c r="A2207" t="n">
+        <v>-19.8961029113522</v>
+      </c>
+      <c r="B2207" t="n">
+        <v>-19.89609796207942</v>
+      </c>
+      <c r="C2207" t="n">
+        <v>13.50891324233384</v>
+      </c>
+    </row>
+    <row r="2208">
+      <c r="A2208" t="n">
+        <v>9.747220500373512</v>
+      </c>
+      <c r="B2208" t="n">
+        <v>9.748954268583869</v>
+      </c>
+      <c r="C2208" t="n">
+        <v>16.04746703319188</v>
+      </c>
+    </row>
+    <row r="2209">
+      <c r="A2209" t="n">
+        <v>9.041427085808614</v>
+      </c>
+      <c r="B2209" t="n">
+        <v>9.043119691663314</v>
+      </c>
+      <c r="C2209" t="n">
+        <v>15.98702527626669</v>
+      </c>
+    </row>
+    <row r="2210">
+      <c r="A2210" t="n">
+        <v>8.335633671243716</v>
+      </c>
+      <c r="B2210" t="n">
+        <v>8.337285114742759</v>
+      </c>
+      <c r="C2210" t="n">
+        <v>15.9265835193415</v>
+      </c>
+    </row>
+    <row r="2211">
+      <c r="A2211" t="n">
+        <v>7.629840256678818</v>
+      </c>
+      <c r="B2211" t="n">
+        <v>7.631450537822205</v>
+      </c>
+      <c r="C2211" t="n">
+        <v>15.8661417624163</v>
+      </c>
+    </row>
+    <row r="2212">
+      <c r="A2212" t="n">
+        <v>6.924046842113921</v>
+      </c>
+      <c r="B2212" t="n">
+        <v>6.92561596090165</v>
+      </c>
+      <c r="C2212" t="n">
+        <v>15.80570000549111</v>
+      </c>
+    </row>
+    <row r="2213">
+      <c r="A2213" t="n">
+        <v>6.218253427549023</v>
+      </c>
+      <c r="B2213" t="n">
+        <v>6.219781383981096</v>
+      </c>
+      <c r="C2213" t="n">
+        <v>15.74525824856592</v>
+      </c>
+    </row>
+    <row r="2214">
+      <c r="A2214" t="n">
+        <v>5.512460012984125</v>
+      </c>
+      <c r="B2214" t="n">
+        <v>5.513946807060542</v>
+      </c>
+      <c r="C2214" t="n">
+        <v>15.68481649164073</v>
+      </c>
+    </row>
+    <row r="2215">
+      <c r="A2215" t="n">
+        <v>4.806666598419227</v>
+      </c>
+      <c r="B2215" t="n">
+        <v>4.808112230139987</v>
+      </c>
+      <c r="C2215" t="n">
+        <v>15.62437473471554</v>
+      </c>
+    </row>
+    <row r="2216">
+      <c r="A2216" t="n">
+        <v>4.100873183854329</v>
+      </c>
+      <c r="B2216" t="n">
+        <v>4.102277653219433</v>
+      </c>
+      <c r="C2216" t="n">
+        <v>15.56393297779034</v>
+      </c>
+    </row>
+    <row r="2217">
+      <c r="A2217" t="n">
+        <v>3.395079769289431</v>
+      </c>
+      <c r="B2217" t="n">
+        <v>3.396443076298878</v>
+      </c>
+      <c r="C2217" t="n">
+        <v>15.50349122086515</v>
+      </c>
+    </row>
+    <row r="2218">
+      <c r="A2218" t="n">
+        <v>2.689286354724533</v>
+      </c>
+      <c r="B2218" t="n">
+        <v>2.690608499378324</v>
+      </c>
+      <c r="C2218" t="n">
+        <v>15.44304946393996</v>
+      </c>
+    </row>
+    <row r="2219">
+      <c r="A2219" t="n">
+        <v>1.983492940159636</v>
+      </c>
+      <c r="B2219" t="n">
+        <v>1.984773922457769</v>
+      </c>
+      <c r="C2219" t="n">
+        <v>15.38260770701477</v>
+      </c>
+    </row>
+    <row r="2220">
+      <c r="A2220" t="n">
+        <v>1.277699525594738</v>
+      </c>
+      <c r="B2220" t="n">
+        <v>1.278939345537215</v>
+      </c>
+      <c r="C2220" t="n">
+        <v>15.32216595008958</v>
+      </c>
+    </row>
+    <row r="2221">
+      <c r="A2221" t="n">
+        <v>0.5719061110298396</v>
+      </c>
+      <c r="B2221" t="n">
+        <v>0.5731047686166604</v>
+      </c>
+      <c r="C2221" t="n">
+        <v>15.26172419316438</v>
+      </c>
+    </row>
+    <row r="2222">
+      <c r="A2222" t="n">
+        <v>-0.1338873035350584</v>
+      </c>
+      <c r="B2222" t="n">
+        <v>-0.132729808303894</v>
+      </c>
+      <c r="C2222" t="n">
+        <v>15.20128243623919</v>
+      </c>
+    </row>
+    <row r="2223">
+      <c r="A2223" t="n">
+        <v>-0.8396807180999564</v>
+      </c>
+      <c r="B2223" t="n">
+        <v>-0.8385643852244485</v>
+      </c>
+      <c r="C2223" t="n">
+        <v>15.140840679314</v>
+      </c>
+    </row>
+    <row r="2224">
+      <c r="A2224" t="n">
+        <v>-1.545474132664854</v>
+      </c>
+      <c r="B2224" t="n">
+        <v>-1.544398962145003</v>
+      </c>
+      <c r="C2224" t="n">
+        <v>15.08039892238881</v>
+      </c>
+    </row>
+    <row r="2225">
+      <c r="A2225" t="n">
+        <v>-2.251267547229752</v>
+      </c>
+      <c r="B2225" t="n">
+        <v>-2.250233539065557</v>
+      </c>
+      <c r="C2225" t="n">
+        <v>15.01995716546362</v>
+      </c>
+    </row>
+    <row r="2226">
+      <c r="A2226" t="n">
+        <v>-2.95706096179465</v>
+      </c>
+      <c r="B2226" t="n">
+        <v>-2.956068115986112</v>
+      </c>
+      <c r="C2226" t="n">
+        <v>14.95951540853843</v>
+      </c>
+    </row>
+    <row r="2227">
+      <c r="A2227" t="n">
+        <v>-3.662854376359548</v>
+      </c>
+      <c r="B2227" t="n">
+        <v>-3.661902692906666</v>
+      </c>
+      <c r="C2227" t="n">
+        <v>14.89907365161323</v>
+      </c>
+    </row>
+    <row r="2228">
+      <c r="A2228" t="n">
+        <v>-4.368647790924446</v>
+      </c>
+      <c r="B2228" t="n">
+        <v>-4.36773726982722</v>
+      </c>
+      <c r="C2228" t="n">
+        <v>14.83863189468804</v>
+      </c>
+    </row>
+    <row r="2229">
+      <c r="A2229" t="n">
+        <v>-5.074441205489344</v>
+      </c>
+      <c r="B2229" t="n">
+        <v>-5.073571846747774</v>
+      </c>
+      <c r="C2229" t="n">
+        <v>14.77819013776285</v>
+      </c>
+    </row>
+    <row r="2230">
+      <c r="A2230" t="n">
+        <v>-5.780234620054242</v>
+      </c>
+      <c r="B2230" t="n">
+        <v>-5.779406423668329</v>
+      </c>
+      <c r="C2230" t="n">
+        <v>14.71774838083766</v>
+      </c>
+    </row>
+    <row r="2231">
+      <c r="A2231" t="n">
+        <v>-6.48602803461914</v>
+      </c>
+      <c r="B2231" t="n">
+        <v>-6.485241000588883</v>
+      </c>
+      <c r="C2231" t="n">
+        <v>14.65730662391247</v>
+      </c>
+    </row>
+    <row r="2232">
+      <c r="A2232" t="n">
+        <v>-7.191821449184038</v>
+      </c>
+      <c r="B2232" t="n">
+        <v>-7.191075577509437</v>
+      </c>
+      <c r="C2232" t="n">
+        <v>14.59686486698728</v>
+      </c>
+    </row>
+    <row r="2233">
+      <c r="A2233" t="n">
+        <v>-7.897614863748935</v>
+      </c>
+      <c r="B2233" t="n">
+        <v>-7.896910154429992</v>
+      </c>
+      <c r="C2233" t="n">
+        <v>14.53642311006208</v>
+      </c>
+    </row>
+    <row r="2234">
+      <c r="A2234" t="n">
+        <v>-8.603408278313834</v>
+      </c>
+      <c r="B2234" t="n">
+        <v>-8.602744731350546</v>
+      </c>
+      <c r="C2234" t="n">
+        <v>14.47598135313689</v>
+      </c>
+    </row>
+    <row r="2235">
+      <c r="A2235" t="n">
+        <v>-9.309201692878732</v>
+      </c>
+      <c r="B2235" t="n">
+        <v>-9.308579308271101</v>
+      </c>
+      <c r="C2235" t="n">
+        <v>14.4155395962117</v>
+      </c>
+    </row>
+    <row r="2236">
+      <c r="A2236" t="n">
+        <v>-10.01499510744363</v>
+      </c>
+      <c r="B2236" t="n">
+        <v>-10.01441388519166</v>
+      </c>
+      <c r="C2236" t="n">
+        <v>14.35509783928651</v>
+      </c>
+    </row>
+    <row r="2237">
+      <c r="A2237" t="n">
+        <v>-10.72078852200853</v>
+      </c>
+      <c r="B2237" t="n">
+        <v>-10.72024846211221</v>
+      </c>
+      <c r="C2237" t="n">
+        <v>14.29465608236132</v>
+      </c>
+    </row>
+    <row r="2238">
+      <c r="A2238" t="n">
+        <v>-11.42658193657343</v>
+      </c>
+      <c r="B2238" t="n">
+        <v>-11.42608303903277</v>
+      </c>
+      <c r="C2238" t="n">
+        <v>14.23421432543613</v>
+      </c>
+    </row>
+    <row r="2239">
+      <c r="A2239" t="n">
+        <v>-12.13237535113832</v>
+      </c>
+      <c r="B2239" t="n">
+        <v>-12.13191761595332</v>
+      </c>
+      <c r="C2239" t="n">
+        <v>14.17377256851094</v>
+      </c>
+    </row>
+    <row r="2240">
+      <c r="A2240" t="n">
+        <v>-12.83816876570322</v>
+      </c>
+      <c r="B2240" t="n">
+        <v>-12.83775219287388</v>
+      </c>
+      <c r="C2240" t="n">
+        <v>14.11333081158575</v>
+      </c>
+    </row>
+    <row r="2241">
+      <c r="A2241" t="n">
+        <v>-13.54396218026812</v>
+      </c>
+      <c r="B2241" t="n">
+        <v>-13.54358676979443</v>
+      </c>
+      <c r="C2241" t="n">
+        <v>14.05288905466056</v>
+      </c>
+    </row>
+    <row r="2242">
+      <c r="A2242" t="n">
+        <v>-14.24975559483302</v>
+      </c>
+      <c r="B2242" t="n">
+        <v>-14.24942134671499</v>
+      </c>
+      <c r="C2242" t="n">
+        <v>13.99244729773537</v>
+      </c>
+    </row>
+    <row r="2243">
+      <c r="A2243" t="n">
+        <v>-14.95554900939791</v>
+      </c>
+      <c r="B2243" t="n">
+        <v>-14.95525592363554</v>
+      </c>
+      <c r="C2243" t="n">
+        <v>13.93200554081018</v>
+      </c>
+    </row>
+    <row r="2244">
+      <c r="A2244" t="n">
+        <v>-15.66134242396281</v>
+      </c>
+      <c r="B2244" t="n">
+        <v>-15.6610905005561</v>
+      </c>
+      <c r="C2244" t="n">
+        <v>13.87156378388499</v>
+      </c>
+    </row>
+    <row r="2245">
+      <c r="A2245" t="n">
+        <v>-16.36713583852771</v>
+      </c>
+      <c r="B2245" t="n">
+        <v>-16.36692507747665</v>
+      </c>
+      <c r="C2245" t="n">
+        <v>13.81112202695979</v>
+      </c>
+    </row>
+    <row r="2246">
+      <c r="A2246" t="n">
+        <v>-17.07292925309261</v>
+      </c>
+      <c r="B2246" t="n">
+        <v>-17.07275965439721</v>
+      </c>
+      <c r="C2246" t="n">
+        <v>13.7506802700346</v>
+      </c>
+    </row>
+    <row r="2247">
+      <c r="A2247" t="n">
+        <v>-17.77872266765751</v>
+      </c>
+      <c r="B2247" t="n">
+        <v>-17.77859423131776</v>
+      </c>
+      <c r="C2247" t="n">
+        <v>13.69023851310941</v>
+      </c>
+    </row>
+    <row r="2248">
+      <c r="A2248" t="n">
+        <v>-18.48451608222241</v>
+      </c>
+      <c r="B2248" t="n">
+        <v>-18.48442880823832</v>
+      </c>
+      <c r="C2248" t="n">
+        <v>13.62979675618422</v>
+      </c>
+    </row>
+    <row r="2249">
+      <c r="A2249" t="n">
+        <v>-19.1903094967873</v>
+      </c>
+      <c r="B2249" t="n">
+        <v>-19.19026338515887</v>
+      </c>
+      <c r="C2249" t="n">
+        <v>13.56935499925903</v>
+      </c>
+    </row>
+    <row r="2250">
+      <c r="A2250" t="n">
+        <v>-19.8961029113522</v>
+      </c>
+      <c r="B2250" t="n">
+        <v>-19.89609796207942</v>
+      </c>
+      <c r="C2250" t="n">
+        <v>13.50891324233384</v>
+      </c>
+    </row>
+    <row r="2251">
+      <c r="A2251" t="n">
+        <v>12.5703941586331</v>
+      </c>
+      <c r="B2251" t="n">
+        <v>12.57229257626609</v>
+      </c>
+      <c r="C2251" t="n">
+        <v>16.28923406089264</v>
+      </c>
+    </row>
+    <row r="2252">
+      <c r="A2252" t="n">
+        <v>10.45301391493841</v>
+      </c>
+      <c r="B2252" t="n">
+        <v>10.45478884550442</v>
+      </c>
+      <c r="C2252" t="n">
+        <v>16.10790879011707</v>
+      </c>
+    </row>
+    <row r="2253">
+      <c r="A2253" t="n">
+        <v>9.747220500373512</v>
+      </c>
+      <c r="B2253" t="n">
+        <v>9.748954268583869</v>
+      </c>
+      <c r="C2253" t="n">
+        <v>16.04746703319188</v>
+      </c>
+    </row>
+    <row r="2254">
+      <c r="A2254" t="n">
+        <v>9.041427085808614</v>
+      </c>
+      <c r="B2254" t="n">
+        <v>9.043119691663314</v>
+      </c>
+      <c r="C2254" t="n">
+        <v>15.98702527626669</v>
+      </c>
+    </row>
+    <row r="2255">
+      <c r="A2255" t="n">
+        <v>8.335633671243716</v>
+      </c>
+      <c r="B2255" t="n">
+        <v>8.337285114742759</v>
+      </c>
+      <c r="C2255" t="n">
+        <v>15.9265835193415</v>
+      </c>
+    </row>
+    <row r="2256">
+      <c r="A2256" t="n">
+        <v>7.629840256678818</v>
+      </c>
+      <c r="B2256" t="n">
+        <v>7.631450537822205</v>
+      </c>
+      <c r="C2256" t="n">
+        <v>15.8661417624163</v>
+      </c>
+    </row>
+    <row r="2257">
+      <c r="A2257" t="n">
+        <v>6.924046842113921</v>
+      </c>
+      <c r="B2257" t="n">
+        <v>6.92561596090165</v>
+      </c>
+      <c r="C2257" t="n">
+        <v>15.80570000549111</v>
+      </c>
+    </row>
+    <row r="2258">
+      <c r="A2258" t="n">
+        <v>6.218253427549023</v>
+      </c>
+      <c r="B2258" t="n">
+        <v>6.219781383981096</v>
+      </c>
+      <c r="C2258" t="n">
+        <v>15.74525824856592</v>
+      </c>
+    </row>
+    <row r="2259">
+      <c r="A2259" t="n">
+        <v>5.512460012984125</v>
+      </c>
+      <c r="B2259" t="n">
+        <v>5.513946807060542</v>
+      </c>
+      <c r="C2259" t="n">
+        <v>15.68481649164073</v>
+      </c>
+    </row>
+    <row r="2260">
+      <c r="A2260" t="n">
+        <v>4.806666598419227</v>
+      </c>
+      <c r="B2260" t="n">
+        <v>4.808112230139987</v>
+      </c>
+      <c r="C2260" t="n">
+        <v>15.62437473471554</v>
+      </c>
+    </row>
+    <row r="2261">
+      <c r="A2261" t="n">
+        <v>4.100873183854329</v>
+      </c>
+      <c r="B2261" t="n">
+        <v>4.102277653219433</v>
+      </c>
+      <c r="C2261" t="n">
+        <v>15.56393297779034</v>
+      </c>
+    </row>
+    <row r="2262">
+      <c r="A2262" t="n">
+        <v>3.395079769289431</v>
+      </c>
+      <c r="B2262" t="n">
+        <v>3.396443076298878</v>
+      </c>
+      <c r="C2262" t="n">
+        <v>15.50349122086515</v>
+      </c>
+    </row>
+    <row r="2263">
+      <c r="A2263" t="n">
+        <v>2.689286354724533</v>
+      </c>
+      <c r="B2263" t="n">
+        <v>2.690608499378324</v>
+      </c>
+      <c r="C2263" t="n">
+        <v>15.44304946393996</v>
+      </c>
+    </row>
+    <row r="2264">
+      <c r="A2264" t="n">
+        <v>1.983492940159636</v>
+      </c>
+      <c r="B2264" t="n">
+        <v>1.984773922457769</v>
+      </c>
+      <c r="C2264" t="n">
+        <v>15.38260770701477</v>
+      </c>
+    </row>
+    <row r="2265">
+      <c r="A2265" t="n">
+        <v>1.277699525594738</v>
+      </c>
+      <c r="B2265" t="n">
+        <v>1.278939345537215</v>
+      </c>
+      <c r="C2265" t="n">
+        <v>15.32216595008958</v>
+      </c>
+    </row>
+    <row r="2266">
+      <c r="A2266" t="n">
+        <v>0.5719061110298396</v>
+      </c>
+      <c r="B2266" t="n">
+        <v>0.5731047686166604</v>
+      </c>
+      <c r="C2266" t="n">
+        <v>15.26172419316438</v>
+      </c>
+    </row>
+    <row r="2267">
+      <c r="A2267" t="n">
+        <v>-0.1338873035350584</v>
+      </c>
+      <c r="B2267" t="n">
+        <v>-0.132729808303894</v>
+      </c>
+      <c r="C2267" t="n">
+        <v>15.20128243623919</v>
+      </c>
+    </row>
+    <row r="2268">
+      <c r="A2268" t="n">
+        <v>-0.8396807180999564</v>
+      </c>
+      <c r="B2268" t="n">
+        <v>-0.8385643852244485</v>
+      </c>
+      <c r="C2268" t="n">
+        <v>15.140840679314</v>
+      </c>
+    </row>
+    <row r="2269">
+      <c r="A2269" t="n">
+        <v>-1.545474132664854</v>
+      </c>
+      <c r="B2269" t="n">
+        <v>-1.544398962145003</v>
+      </c>
+      <c r="C2269" t="n">
+        <v>15.08039892238881</v>
+      </c>
+    </row>
+    <row r="2270">
+      <c r="A2270" t="n">
+        <v>-2.251267547229752</v>
+      </c>
+      <c r="B2270" t="n">
+        <v>-2.250233539065557</v>
+      </c>
+      <c r="C2270" t="n">
+        <v>15.01995716546362</v>
+      </c>
+    </row>
+    <row r="2271">
+      <c r="A2271" t="n">
+        <v>-2.95706096179465</v>
+      </c>
+      <c r="B2271" t="n">
+        <v>-2.956068115986112</v>
+      </c>
+      <c r="C2271" t="n">
+        <v>14.95951540853843</v>
+      </c>
+    </row>
+    <row r="2272">
+      <c r="A2272" t="n">
+        <v>-3.662854376359548</v>
+      </c>
+      <c r="B2272" t="n">
+        <v>-3.661902692906666</v>
+      </c>
+      <c r="C2272" t="n">
+        <v>14.89907365161323</v>
+      </c>
+    </row>
+    <row r="2273">
+      <c r="A2273" t="n">
+        <v>-4.368647790924446</v>
+      </c>
+      <c r="B2273" t="n">
+        <v>-4.36773726982722</v>
+      </c>
+      <c r="C2273" t="n">
+        <v>14.83863189468804</v>
+      </c>
+    </row>
+    <row r="2274">
+      <c r="A2274" t="n">
+        <v>-5.074441205489344</v>
+      </c>
+      <c r="B2274" t="n">
+        <v>-5.073571846747774</v>
+      </c>
+      <c r="C2274" t="n">
+        <v>14.77819013776285</v>
+      </c>
+    </row>
+    <row r="2275">
+      <c r="A2275" t="n">
+        <v>-5.780234620054242</v>
+      </c>
+      <c r="B2275" t="n">
+        <v>-5.779406423668329</v>
+      </c>
+      <c r="C2275" t="n">
+        <v>14.71774838083766</v>
+      </c>
+    </row>
+    <row r="2276">
+      <c r="A2276" t="n">
+        <v>-6.48602803461914</v>
+      </c>
+      <c r="B2276" t="n">
+        <v>-6.485241000588883</v>
+      </c>
+      <c r="C2276" t="n">
+        <v>14.65730662391247</v>
+      </c>
+    </row>
+    <row r="2277">
+      <c r="A2277" t="n">
+        <v>-7.191821449184038</v>
+      </c>
+      <c r="B2277" t="n">
+        <v>-7.191075577509437</v>
+      </c>
+      <c r="C2277" t="n">
+        <v>14.59686486698728</v>
+      </c>
+    </row>
+    <row r="2278">
+      <c r="A2278" t="n">
+        <v>-7.897614863748935</v>
+      </c>
+      <c r="B2278" t="n">
+        <v>-7.896910154429992</v>
+      </c>
+      <c r="C2278" t="n">
+        <v>14.53642311006208</v>
+      </c>
+    </row>
+    <row r="2279">
+      <c r="A2279" t="n">
+        <v>-8.603408278313834</v>
+      </c>
+      <c r="B2279" t="n">
+        <v>-8.602744731350546</v>
+      </c>
+      <c r="C2279" t="n">
+        <v>14.47598135313689</v>
+      </c>
+    </row>
+    <row r="2280">
+      <c r="A2280" t="n">
+        <v>-9.309201692878732</v>
+      </c>
+      <c r="B2280" t="n">
+        <v>-9.308579308271101</v>
+      </c>
+      <c r="C2280" t="n">
+        <v>14.4155395962117</v>
+      </c>
+    </row>
+    <row r="2281">
+      <c r="A2281" t="n">
+        <v>-10.01499510744363</v>
+      </c>
+      <c r="B2281" t="n">
+        <v>-10.01441388519166</v>
+      </c>
+      <c r="C2281" t="n">
+        <v>14.35509783928651</v>
+      </c>
+    </row>
+    <row r="2282">
+      <c r="A2282" t="n">
+        <v>-10.72078852200853</v>
+      </c>
+      <c r="B2282" t="n">
+        <v>-10.72024846211221</v>
+      </c>
+      <c r="C2282" t="n">
+        <v>14.29465608236132</v>
+      </c>
+    </row>
+    <row r="2283">
+      <c r="A2283" t="n">
+        <v>-11.42658193657343</v>
+      </c>
+      <c r="B2283" t="n">
+        <v>-11.42608303903277</v>
+      </c>
+      <c r="C2283" t="n">
+        <v>14.23421432543613</v>
+      </c>
+    </row>
+    <row r="2284">
+      <c r="A2284" t="n">
+        <v>-12.13237535113832</v>
+      </c>
+      <c r="B2284" t="n">
+        <v>-12.13191761595332</v>
+      </c>
+      <c r="C2284" t="n">
+        <v>14.17377256851094</v>
+      </c>
+    </row>
+    <row r="2285">
+      <c r="A2285" t="n">
+        <v>-12.83816876570322</v>
+      </c>
+      <c r="B2285" t="n">
+        <v>-12.83775219287388</v>
+      </c>
+      <c r="C2285" t="n">
+        <v>14.11333081158575</v>
+      </c>
+    </row>
+    <row r="2286">
+      <c r="A2286" t="n">
+        <v>-13.54396218026812</v>
+      </c>
+      <c r="B2286" t="n">
+        <v>-13.54358676979443</v>
+      </c>
+      <c r="C2286" t="n">
+        <v>14.05288905466056</v>
+      </c>
+    </row>
+    <row r="2287">
+      <c r="A2287" t="n">
+        <v>-14.24975559483302</v>
+      </c>
+      <c r="B2287" t="n">
+        <v>-14.24942134671499</v>
+      </c>
+      <c r="C2287" t="n">
+        <v>13.99244729773537</v>
+      </c>
+    </row>
+    <row r="2288">
+      <c r="A2288" t="n">
+        <v>-14.95554900939791</v>
+      </c>
+      <c r="B2288" t="n">
+        <v>-14.95525592363554</v>
+      </c>
+      <c r="C2288" t="n">
+        <v>13.93200554081018</v>
+      </c>
+    </row>
+    <row r="2289">
+      <c r="A2289" t="n">
+        <v>-15.66134242396281</v>
+      </c>
+      <c r="B2289" t="n">
+        <v>-15.6610905005561</v>
+      </c>
+      <c r="C2289" t="n">
+        <v>13.87156378388499</v>
+      </c>
+    </row>
+    <row r="2290">
+      <c r="A2290" t="n">
+        <v>-16.36713583852771</v>
+      </c>
+      <c r="B2290" t="n">
+        <v>-16.36692507747665</v>
+      </c>
+      <c r="C2290" t="n">
+        <v>13.81112202695979</v>
+      </c>
+    </row>
+    <row r="2291">
+      <c r="A2291" t="n">
+        <v>-17.07292925309261</v>
+      </c>
+      <c r="B2291" t="n">
+        <v>-17.07275965439721</v>
+      </c>
+      <c r="C2291" t="n">
+        <v>13.7506802700346</v>
+      </c>
+    </row>
+    <row r="2292">
+      <c r="A2292" t="n">
+        <v>-17.77872266765751</v>
+      </c>
+      <c r="B2292" t="n">
+        <v>-17.77859423131776</v>
+      </c>
+      <c r="C2292" t="n">
+        <v>13.69023851310941</v>
+      </c>
+    </row>
+    <row r="2293">
+      <c r="A2293" t="n">
+        <v>-18.48451608222241</v>
+      </c>
+      <c r="B2293" t="n">
+        <v>-18.48442880823832</v>
+      </c>
+      <c r="C2293" t="n">
+        <v>13.62979675618422</v>
+      </c>
+    </row>
+    <row r="2294">
+      <c r="A2294" t="n">
+        <v>-19.1903094967873</v>
+      </c>
+      <c r="B2294" t="n">
+        <v>-19.19026338515887</v>
+      </c>
+      <c r="C2294" t="n">
+        <v>13.56935499925903</v>
+      </c>
+    </row>
+    <row r="2295">
+      <c r="A2295" t="n">
+        <v>-19.8961029113522</v>
+      </c>
+      <c r="B2295" t="n">
+        <v>-19.89609796207942</v>
+      </c>
+      <c r="C2295" t="n">
+        <v>13.50891324233384</v>
+      </c>
+    </row>
+    <row r="2296">
+      <c r="A2296" t="n">
+        <v>9.747220500373512</v>
+      </c>
+      <c r="B2296" t="n">
+        <v>9.748954268583869</v>
+      </c>
+      <c r="C2296" t="n">
+        <v>16.04746703319188</v>
+      </c>
+    </row>
+    <row r="2297">
+      <c r="A2297" t="n">
+        <v>9.041427085808614</v>
+      </c>
+      <c r="B2297" t="n">
+        <v>9.043119691663314</v>
+      </c>
+      <c r="C2297" t="n">
+        <v>15.98702527626669</v>
+      </c>
+    </row>
+    <row r="2298">
+      <c r="A2298" t="n">
+        <v>8.335633671243716</v>
+      </c>
+      <c r="B2298" t="n">
+        <v>8.337285114742759</v>
+      </c>
+      <c r="C2298" t="n">
+        <v>15.9265835193415</v>
+      </c>
+    </row>
+    <row r="2299">
+      <c r="A2299" t="n">
+        <v>7.629840256678818</v>
+      </c>
+      <c r="B2299" t="n">
+        <v>7.631450537822205</v>
+      </c>
+      <c r="C2299" t="n">
+        <v>15.8661417624163</v>
+      </c>
+    </row>
+    <row r="2300">
+      <c r="A2300" t="n">
+        <v>6.924046842113921</v>
+      </c>
+      <c r="B2300" t="n">
+        <v>6.92561596090165</v>
+      </c>
+      <c r="C2300" t="n">
+        <v>15.80570000549111</v>
+      </c>
+    </row>
+    <row r="2301">
+      <c r="A2301" t="n">
+        <v>6.218253427549023</v>
+      </c>
+      <c r="B2301" t="n">
+        <v>6.219781383981096</v>
+      </c>
+      <c r="C2301" t="n">
+        <v>15.74525824856592</v>
+      </c>
+    </row>
+    <row r="2302">
+      <c r="A2302" t="n">
+        <v>5.512460012984125</v>
+      </c>
+      <c r="B2302" t="n">
+        <v>5.513946807060542</v>
+      </c>
+      <c r="C2302" t="n">
+        <v>15.68481649164073</v>
+      </c>
+    </row>
+    <row r="2303">
+      <c r="A2303" t="n">
+        <v>4.806666598419227</v>
+      </c>
+      <c r="B2303" t="n">
+        <v>4.808112230139987</v>
+      </c>
+      <c r="C2303" t="n">
+        <v>15.62437473471554</v>
+      </c>
+    </row>
+    <row r="2304">
+      <c r="A2304" t="n">
+        <v>4.100873183854329</v>
+      </c>
+      <c r="B2304" t="n">
+        <v>4.102277653219433</v>
+      </c>
+      <c r="C2304" t="n">
+        <v>15.56393297779034</v>
+      </c>
+    </row>
+    <row r="2305">
+      <c r="A2305" t="n">
+        <v>3.395079769289431</v>
+      </c>
+      <c r="B2305" t="n">
+        <v>3.396443076298878</v>
+      </c>
+      <c r="C2305" t="n">
+        <v>15.50349122086515</v>
+      </c>
+    </row>
+    <row r="2306">
+      <c r="A2306" t="n">
+        <v>2.689286354724533</v>
+      </c>
+      <c r="B2306" t="n">
+        <v>2.690608499378324</v>
+      </c>
+      <c r="C2306" t="n">
+        <v>15.44304946393996</v>
+      </c>
+    </row>
+    <row r="2307">
+      <c r="A2307" t="n">
+        <v>1.983492940159636</v>
+      </c>
+      <c r="B2307" t="n">
+        <v>1.984773922457769</v>
+      </c>
+      <c r="C2307" t="n">
+        <v>15.38260770701477</v>
+      </c>
+    </row>
+    <row r="2308">
+      <c r="A2308" t="n">
+        <v>1.277699525594738</v>
+      </c>
+      <c r="B2308" t="n">
+        <v>1.278939345537215</v>
+      </c>
+      <c r="C2308" t="n">
+        <v>15.32216595008958</v>
+      </c>
+    </row>
+    <row r="2309">
+      <c r="A2309" t="n">
+        <v>0.5719061110298396</v>
+      </c>
+      <c r="B2309" t="n">
+        <v>0.5731047686166604</v>
+      </c>
+      <c r="C2309" t="n">
+        <v>15.26172419316438</v>
+      </c>
+    </row>
+    <row r="2310">
+      <c r="A2310" t="n">
+        <v>-0.1338873035350584</v>
+      </c>
+      <c r="B2310" t="n">
+        <v>-0.132729808303894</v>
+      </c>
+      <c r="C2310" t="n">
+        <v>15.20128243623919</v>
+      </c>
+    </row>
+    <row r="2311">
+      <c r="A2311" t="n">
+        <v>-0.8396807180999564</v>
+      </c>
+      <c r="B2311" t="n">
+        <v>-0.8385643852244485</v>
+      </c>
+      <c r="C2311" t="n">
+        <v>15.140840679314</v>
+      </c>
+    </row>
+    <row r="2312">
+      <c r="A2312" t="n">
+        <v>-1.545474132664854</v>
+      </c>
+      <c r="B2312" t="n">
+        <v>-1.544398962145003</v>
+      </c>
+      <c r="C2312" t="n">
+        <v>15.08039892238881</v>
+      </c>
+    </row>
+    <row r="2313">
+      <c r="A2313" t="n">
+        <v>-2.251267547229752</v>
+      </c>
+      <c r="B2313" t="n">
+        <v>-2.250233539065557</v>
+      </c>
+      <c r="C2313" t="n">
+        <v>15.01995716546362</v>
+      </c>
+    </row>
+    <row r="2314">
+      <c r="A2314" t="n">
+        <v>-2.95706096179465</v>
+      </c>
+      <c r="B2314" t="n">
+        <v>-2.956068115986112</v>
+      </c>
+      <c r="C2314" t="n">
+        <v>14.95951540853843</v>
+      </c>
+    </row>
+    <row r="2315">
+      <c r="A2315" t="n">
+        <v>-3.662854376359548</v>
+      </c>
+      <c r="B2315" t="n">
+        <v>-3.661902692906666</v>
+      </c>
+      <c r="C2315" t="n">
+        <v>14.89907365161323</v>
+      </c>
+    </row>
+    <row r="2316">
+      <c r="A2316" t="n">
+        <v>-4.368647790924446</v>
+      </c>
+      <c r="B2316" t="n">
+        <v>-4.36773726982722</v>
+      </c>
+      <c r="C2316" t="n">
+        <v>14.83863189468804</v>
+      </c>
+    </row>
+    <row r="2317">
+      <c r="A2317" t="n">
+        <v>-5.074441205489344</v>
+      </c>
+      <c r="B2317" t="n">
+        <v>-5.073571846747774</v>
+      </c>
+      <c r="C2317" t="n">
+        <v>14.77819013776285</v>
+      </c>
+    </row>
+    <row r="2318">
+      <c r="A2318" t="n">
+        <v>-5.780234620054242</v>
+      </c>
+      <c r="B2318" t="n">
+        <v>-5.779406423668329</v>
+      </c>
+      <c r="C2318" t="n">
+        <v>14.71774838083766</v>
+      </c>
+    </row>
+    <row r="2319">
+      <c r="A2319" t="n">
+        <v>-6.48602803461914</v>
+      </c>
+      <c r="B2319" t="n">
+        <v>-6.485241000588883</v>
+      </c>
+      <c r="C2319" t="n">
+        <v>14.65730662391247</v>
+      </c>
+    </row>
+    <row r="2320">
+      <c r="A2320" t="n">
+        <v>-7.191821449184038</v>
+      </c>
+      <c r="B2320" t="n">
+        <v>-7.191075577509437</v>
+      </c>
+      <c r="C2320" t="n">
+        <v>14.59686486698728</v>
+      </c>
+    </row>
+    <row r="2321">
+      <c r="A2321" t="n">
+        <v>-7.897614863748935</v>
+      </c>
+      <c r="B2321" t="n">
+        <v>-7.896910154429992</v>
+      </c>
+      <c r="C2321" t="n">
+        <v>14.53642311006208</v>
+      </c>
+    </row>
+    <row r="2322">
+      <c r="A2322" t="n">
+        <v>-8.603408278313834</v>
+      </c>
+      <c r="B2322" t="n">
+        <v>-8.602744731350546</v>
+      </c>
+      <c r="C2322" t="n">
+        <v>14.47598135313689</v>
+      </c>
+    </row>
+    <row r="2323">
+      <c r="A2323" t="n">
+        <v>-9.309201692878732</v>
+      </c>
+      <c r="B2323" t="n">
+        <v>-9.308579308271101</v>
+      </c>
+      <c r="C2323" t="n">
+        <v>14.4155395962117</v>
+      </c>
+    </row>
+    <row r="2324">
+      <c r="A2324" t="n">
+        <v>-10.01499510744363</v>
+      </c>
+      <c r="B2324" t="n">
+        <v>-10.01441388519166</v>
+      </c>
+      <c r="C2324" t="n">
+        <v>14.35509783928651</v>
+      </c>
+    </row>
+    <row r="2325">
+      <c r="A2325" t="n">
+        <v>-10.72078852200853</v>
+      </c>
+      <c r="B2325" t="n">
+        <v>-10.72024846211221</v>
+      </c>
+      <c r="C2325" t="n">
+        <v>14.29465608236132</v>
+      </c>
+    </row>
+    <row r="2326">
+      <c r="A2326" t="n">
+        <v>-11.42658193657343</v>
+      </c>
+      <c r="B2326" t="n">
+        <v>-11.42608303903277</v>
+      </c>
+      <c r="C2326" t="n">
+        <v>14.23421432543613</v>
+      </c>
+    </row>
+    <row r="2327">
+      <c r="A2327" t="n">
+        <v>-12.13237535113832</v>
+      </c>
+      <c r="B2327" t="n">
+        <v>-12.13191761595332</v>
+      </c>
+      <c r="C2327" t="n">
+        <v>14.17377256851094</v>
+      </c>
+    </row>
+    <row r="2328">
+      <c r="A2328" t="n">
+        <v>-12.83816876570322</v>
+      </c>
+      <c r="B2328" t="n">
+        <v>-12.83775219287388</v>
+      </c>
+      <c r="C2328" t="n">
+        <v>14.11333081158575</v>
+      </c>
+    </row>
+    <row r="2329">
+      <c r="A2329" t="n">
+        <v>-13.54396218026812</v>
+      </c>
+      <c r="B2329" t="n">
+        <v>-13.54358676979443</v>
+      </c>
+      <c r="C2329" t="n">
+        <v>14.05288905466056</v>
+      </c>
+    </row>
+    <row r="2330">
+      <c r="A2330" t="n">
+        <v>-14.24975559483302</v>
+      </c>
+      <c r="B2330" t="n">
+        <v>-14.24942134671499</v>
+      </c>
+      <c r="C2330" t="n">
+        <v>13.99244729773537</v>
+      </c>
+    </row>
+    <row r="2331">
+      <c r="A2331" t="n">
+        <v>-14.95554900939791</v>
+      </c>
+      <c r="B2331" t="n">
+        <v>-14.95525592363554</v>
+      </c>
+      <c r="C2331" t="n">
+        <v>13.93200554081018</v>
+      </c>
+    </row>
+    <row r="2332">
+      <c r="A2332" t="n">
+        <v>-15.66134242396281</v>
+      </c>
+      <c r="B2332" t="n">
+        <v>-15.6610905005561</v>
+      </c>
+      <c r="C2332" t="n">
+        <v>13.87156378388499</v>
+      </c>
+    </row>
+    <row r="2333">
+      <c r="A2333" t="n">
+        <v>-16.36713583852771</v>
+      </c>
+      <c r="B2333" t="n">
+        <v>-16.36692507747665</v>
+      </c>
+      <c r="C2333" t="n">
+        <v>13.81112202695979</v>
+      </c>
+    </row>
+    <row r="2334">
+      <c r="A2334" t="n">
+        <v>-17.07292925309261</v>
+      </c>
+      <c r="B2334" t="n">
+        <v>-17.07275965439721</v>
+      </c>
+      <c r="C2334" t="n">
+        <v>13.7506802700346</v>
+      </c>
+    </row>
+    <row r="2335">
+      <c r="A2335" t="n">
+        <v>-17.77872266765751</v>
+      </c>
+      <c r="B2335" t="n">
+        <v>-17.77859423131776</v>
+      </c>
+      <c r="C2335" t="n">
+        <v>13.69023851310941</v>
+      </c>
+    </row>
+    <row r="2336">
+      <c r="A2336" t="n">
+        <v>-18.48451608222241</v>
+      </c>
+      <c r="B2336" t="n">
+        <v>-18.48442880823832</v>
+      </c>
+      <c r="C2336" t="n">
+        <v>13.62979675618422</v>
+      </c>
+    </row>
+    <row r="2337">
+      <c r="A2337" t="n">
+        <v>-19.1903094967873</v>
+      </c>
+      <c r="B2337" t="n">
+        <v>-19.19026338515887</v>
+      </c>
+      <c r="C2337" t="n">
+        <v>13.56935499925903</v>
+      </c>
+    </row>
+    <row r="2338">
+      <c r="A2338" t="n">
+        <v>-19.8961029113522</v>
+      </c>
+      <c r="B2338" t="n">
+        <v>-19.89609796207942</v>
+      </c>
+      <c r="C2338" t="n">
+        <v>13.50891324233384</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
idk what it did but its not broken now
</commit_message>
<xml_diff>
--- a/src/path_planning/test_scripts/Testing.xlsx
+++ b/src/path_planning/test_scripts/Testing.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2338"/>
+  <dimension ref="A1:C2381"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -26138,6 +26138,479 @@
         <v>13.50891324233384</v>
       </c>
     </row>
+    <row r="2339">
+      <c r="A2339" t="n">
+        <v>9.73745786833307</v>
+      </c>
+      <c r="B2339" t="n">
+        <v>9.737043825499235</v>
+      </c>
+      <c r="C2339" t="n">
+        <v>16.19082042100107</v>
+      </c>
+    </row>
+    <row r="2340">
+      <c r="A2340" t="n">
+        <v>9.031789155793497</v>
+      </c>
+      <c r="B2340" t="n">
+        <v>9.031384911842718</v>
+      </c>
+      <c r="C2340" t="n">
+        <v>16.12696773335329</v>
+      </c>
+    </row>
+    <row r="2341">
+      <c r="A2341" t="n">
+        <v>8.326120443253924</v>
+      </c>
+      <c r="B2341" t="n">
+        <v>8.325725998186201</v>
+      </c>
+      <c r="C2341" t="n">
+        <v>16.0631150457055</v>
+      </c>
+    </row>
+    <row r="2342">
+      <c r="A2342" t="n">
+        <v>7.62045173071435</v>
+      </c>
+      <c r="B2342" t="n">
+        <v>7.620067084529683</v>
+      </c>
+      <c r="C2342" t="n">
+        <v>15.99926235805772</v>
+      </c>
+    </row>
+    <row r="2343">
+      <c r="A2343" t="n">
+        <v>6.914783018174777</v>
+      </c>
+      <c r="B2343" t="n">
+        <v>6.914408170873166</v>
+      </c>
+      <c r="C2343" t="n">
+        <v>15.93540967040993</v>
+      </c>
+    </row>
+    <row r="2344">
+      <c r="A2344" t="n">
+        <v>6.209114305635204</v>
+      </c>
+      <c r="B2344" t="n">
+        <v>6.208749257216649</v>
+      </c>
+      <c r="C2344" t="n">
+        <v>15.87155698276215</v>
+      </c>
+    </row>
+    <row r="2345">
+      <c r="A2345" t="n">
+        <v>5.503445593095631</v>
+      </c>
+      <c r="B2345" t="n">
+        <v>5.503090343560132</v>
+      </c>
+      <c r="C2345" t="n">
+        <v>15.80770429511436</v>
+      </c>
+    </row>
+    <row r="2346">
+      <c r="A2346" t="n">
+        <v>4.797776880556057</v>
+      </c>
+      <c r="B2346" t="n">
+        <v>4.797431429903615</v>
+      </c>
+      <c r="C2346" t="n">
+        <v>15.74385160746658</v>
+      </c>
+    </row>
+    <row r="2347">
+      <c r="A2347" t="n">
+        <v>4.092108168016484</v>
+      </c>
+      <c r="B2347" t="n">
+        <v>4.091772516247099</v>
+      </c>
+      <c r="C2347" t="n">
+        <v>15.67999891981879</v>
+      </c>
+    </row>
+    <row r="2348">
+      <c r="A2348" t="n">
+        <v>3.386439455476911</v>
+      </c>
+      <c r="B2348" t="n">
+        <v>3.386113602590582</v>
+      </c>
+      <c r="C2348" t="n">
+        <v>15.61614623217101</v>
+      </c>
+    </row>
+    <row r="2349">
+      <c r="A2349" t="n">
+        <v>2.680770742937337</v>
+      </c>
+      <c r="B2349" t="n">
+        <v>2.680454688934065</v>
+      </c>
+      <c r="C2349" t="n">
+        <v>15.55229354452322</v>
+      </c>
+    </row>
+    <row r="2350">
+      <c r="A2350" t="n">
+        <v>1.975102030397764</v>
+      </c>
+      <c r="B2350" t="n">
+        <v>1.974795775277549</v>
+      </c>
+      <c r="C2350" t="n">
+        <v>15.48844085687544</v>
+      </c>
+    </row>
+    <row r="2351">
+      <c r="A2351" t="n">
+        <v>1.269433317858191</v>
+      </c>
+      <c r="B2351" t="n">
+        <v>1.269136861621032</v>
+      </c>
+      <c r="C2351" t="n">
+        <v>15.42458816922765</v>
+      </c>
+    </row>
+    <row r="2352">
+      <c r="A2352" t="n">
+        <v>0.5637646053186174</v>
+      </c>
+      <c r="B2352" t="n">
+        <v>0.5634779479645151</v>
+      </c>
+      <c r="C2352" t="n">
+        <v>15.36073548157987</v>
+      </c>
+    </row>
+    <row r="2353">
+      <c r="A2353" t="n">
+        <v>-0.1419041072209559</v>
+      </c>
+      <c r="B2353" t="n">
+        <v>-0.1421809656920016</v>
+      </c>
+      <c r="C2353" t="n">
+        <v>15.29688279393208</v>
+      </c>
+    </row>
+    <row r="2354">
+      <c r="A2354" t="n">
+        <v>-0.8475728197605292</v>
+      </c>
+      <c r="B2354" t="n">
+        <v>-0.8478398793485182</v>
+      </c>
+      <c r="C2354" t="n">
+        <v>15.2330301062843</v>
+      </c>
+    </row>
+    <row r="2355">
+      <c r="A2355" t="n">
+        <v>-1.553241532300103</v>
+      </c>
+      <c r="B2355" t="n">
+        <v>-1.553498793005035</v>
+      </c>
+      <c r="C2355" t="n">
+        <v>15.16917741863651</v>
+      </c>
+    </row>
+    <row r="2356">
+      <c r="A2356" t="n">
+        <v>-2.258910244839676</v>
+      </c>
+      <c r="B2356" t="n">
+        <v>-2.259157706661552</v>
+      </c>
+      <c r="C2356" t="n">
+        <v>15.10532473098873</v>
+      </c>
+    </row>
+    <row r="2357">
+      <c r="A2357" t="n">
+        <v>-2.964578957379249</v>
+      </c>
+      <c r="B2357" t="n">
+        <v>-2.964816620318068</v>
+      </c>
+      <c r="C2357" t="n">
+        <v>15.04147204334094</v>
+      </c>
+    </row>
+    <row r="2358">
+      <c r="A2358" t="n">
+        <v>-3.670247669918822</v>
+      </c>
+      <c r="B2358" t="n">
+        <v>-3.670475533974585</v>
+      </c>
+      <c r="C2358" t="n">
+        <v>14.97761935569316</v>
+      </c>
+    </row>
+    <row r="2359">
+      <c r="A2359" t="n">
+        <v>-4.375916382458396</v>
+      </c>
+      <c r="B2359" t="n">
+        <v>-4.376134447631102</v>
+      </c>
+      <c r="C2359" t="n">
+        <v>14.91376666804537</v>
+      </c>
+    </row>
+    <row r="2360">
+      <c r="A2360" t="n">
+        <v>-5.081585094997969</v>
+      </c>
+      <c r="B2360" t="n">
+        <v>-5.081793361287619</v>
+      </c>
+      <c r="C2360" t="n">
+        <v>14.84991398039759</v>
+      </c>
+    </row>
+    <row r="2361">
+      <c r="A2361" t="n">
+        <v>-5.787253807537542</v>
+      </c>
+      <c r="B2361" t="n">
+        <v>-5.787452274944135</v>
+      </c>
+      <c r="C2361" t="n">
+        <v>14.7860612927498</v>
+      </c>
+    </row>
+    <row r="2362">
+      <c r="A2362" t="n">
+        <v>-6.492922520077116</v>
+      </c>
+      <c r="B2362" t="n">
+        <v>-6.493111188600652</v>
+      </c>
+      <c r="C2362" t="n">
+        <v>14.72220860510201</v>
+      </c>
+    </row>
+    <row r="2363">
+      <c r="A2363" t="n">
+        <v>-7.198591232616689</v>
+      </c>
+      <c r="B2363" t="n">
+        <v>-7.198770102257169</v>
+      </c>
+      <c r="C2363" t="n">
+        <v>14.65835591745423</v>
+      </c>
+    </row>
+    <row r="2364">
+      <c r="A2364" t="n">
+        <v>-7.904259945156262</v>
+      </c>
+      <c r="B2364" t="n">
+        <v>-7.904429015913685</v>
+      </c>
+      <c r="C2364" t="n">
+        <v>14.59450322980644</v>
+      </c>
+    </row>
+    <row r="2365">
+      <c r="A2365" t="n">
+        <v>-8.609928657695836</v>
+      </c>
+      <c r="B2365" t="n">
+        <v>-8.610087929570202</v>
+      </c>
+      <c r="C2365" t="n">
+        <v>14.53065054215866</v>
+      </c>
+    </row>
+    <row r="2366">
+      <c r="A2366" t="n">
+        <v>-9.315597370235409</v>
+      </c>
+      <c r="B2366" t="n">
+        <v>-9.315746843226719</v>
+      </c>
+      <c r="C2366" t="n">
+        <v>14.46679785451087</v>
+      </c>
+    </row>
+    <row r="2367">
+      <c r="A2367" t="n">
+        <v>-10.02126608277498</v>
+      </c>
+      <c r="B2367" t="n">
+        <v>-10.02140575688324</v>
+      </c>
+      <c r="C2367" t="n">
+        <v>14.40294516686309</v>
+      </c>
+    </row>
+    <row r="2368">
+      <c r="A2368" t="n">
+        <v>-10.72693479531456</v>
+      </c>
+      <c r="B2368" t="n">
+        <v>-10.72706467053975</v>
+      </c>
+      <c r="C2368" t="n">
+        <v>14.3390924792153</v>
+      </c>
+    </row>
+    <row r="2369">
+      <c r="A2369" t="n">
+        <v>-11.43260350785413</v>
+      </c>
+      <c r="B2369" t="n">
+        <v>-11.43272358419627</v>
+      </c>
+      <c r="C2369" t="n">
+        <v>14.27523979156751</v>
+      </c>
+    </row>
+    <row r="2370">
+      <c r="A2370" t="n">
+        <v>-12.1382722203937</v>
+      </c>
+      <c r="B2370" t="n">
+        <v>-12.13838249785279</v>
+      </c>
+      <c r="C2370" t="n">
+        <v>14.21138710391973</v>
+      </c>
+    </row>
+    <row r="2371">
+      <c r="A2371" t="n">
+        <v>-12.84394093293328</v>
+      </c>
+      <c r="B2371" t="n">
+        <v>-12.84404141150931</v>
+      </c>
+      <c r="C2371" t="n">
+        <v>14.14753441627194</v>
+      </c>
+    </row>
+    <row r="2372">
+      <c r="A2372" t="n">
+        <v>-13.54960964547285</v>
+      </c>
+      <c r="B2372" t="n">
+        <v>-13.54970032516582</v>
+      </c>
+      <c r="C2372" t="n">
+        <v>14.08368172862416</v>
+      </c>
+    </row>
+    <row r="2373">
+      <c r="A2373" t="n">
+        <v>-14.25527835801242</v>
+      </c>
+      <c r="B2373" t="n">
+        <v>-14.25535923882234</v>
+      </c>
+      <c r="C2373" t="n">
+        <v>14.01982904097637</v>
+      </c>
+    </row>
+    <row r="2374">
+      <c r="A2374" t="n">
+        <v>-14.960947070552</v>
+      </c>
+      <c r="B2374" t="n">
+        <v>-14.96101815247886</v>
+      </c>
+      <c r="C2374" t="n">
+        <v>13.95597635332859</v>
+      </c>
+    </row>
+    <row r="2375">
+      <c r="A2375" t="n">
+        <v>-15.66661578309157</v>
+      </c>
+      <c r="B2375" t="n">
+        <v>-15.66667706613537</v>
+      </c>
+      <c r="C2375" t="n">
+        <v>13.8921236656808</v>
+      </c>
+    </row>
+    <row r="2376">
+      <c r="A2376" t="n">
+        <v>-16.37228449563114</v>
+      </c>
+      <c r="B2376" t="n">
+        <v>-16.37233597979189</v>
+      </c>
+      <c r="C2376" t="n">
+        <v>13.82827097803302</v>
+      </c>
+    </row>
+    <row r="2377">
+      <c r="A2377" t="n">
+        <v>-17.07795320817072</v>
+      </c>
+      <c r="B2377" t="n">
+        <v>-17.07799489344841</v>
+      </c>
+      <c r="C2377" t="n">
+        <v>13.76441829038523</v>
+      </c>
+    </row>
+    <row r="2378">
+      <c r="A2378" t="n">
+        <v>-17.78362192071029</v>
+      </c>
+      <c r="B2378" t="n">
+        <v>-17.78365380710493</v>
+      </c>
+      <c r="C2378" t="n">
+        <v>13.70056560273744</v>
+      </c>
+    </row>
+    <row r="2379">
+      <c r="A2379" t="n">
+        <v>-18.48929063324986</v>
+      </c>
+      <c r="B2379" t="n">
+        <v>-18.48931272076144</v>
+      </c>
+      <c r="C2379" t="n">
+        <v>13.63671291508966</v>
+      </c>
+    </row>
+    <row r="2380">
+      <c r="A2380" t="n">
+        <v>-19.19495934578944</v>
+      </c>
+      <c r="B2380" t="n">
+        <v>-19.19497163441796</v>
+      </c>
+      <c r="C2380" t="n">
+        <v>13.57286022744187</v>
+      </c>
+    </row>
+    <row r="2381">
+      <c r="A2381" t="n">
+        <v>-19.90062805832901</v>
+      </c>
+      <c r="B2381" t="n">
+        <v>-19.90063054807447</v>
+      </c>
+      <c r="C2381" t="n">
+        <v>13.50900753979409</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>